<commit_message>
Added hour to the time sheet
</commit_message>
<xml_diff>
--- a/src/assets/timesheets/time-SP_TimeSheet_Laxmi.xlsx
+++ b/src/assets/timesheets/time-SP_TimeSheet_Laxmi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laxmi\Desktop\College\Projects\senior-project-website\src\assets\timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8012A23-8C43-4246-AFA6-DB976D83D23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBFAC97-83B0-40B8-B76F-D867942FA53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{28D9A5AF-D39E-412B-BBB9-56A34DC76385}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{28D9A5AF-D39E-412B-BBB9-56A34DC76385}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Friday</t>
+  </si>
+  <si>
+    <t>React spike</t>
   </si>
 </sst>
 </file>
@@ -125,13 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -469,18 +470,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF860194-344E-4D78-94A8-8421A58AF9C1}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="142.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="142.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -494,927 +495,840 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>45556</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>45557</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>45558</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>45559</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>45560</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>45561</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>45562</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>45563</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>45564</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>45565</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>45566</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>45567</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>45568</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>45569</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>45570</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>45571</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>45572</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>45573</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>45574</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>45575</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>45576</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>45577</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>45578</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>45579</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>45580</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>45581</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>45582</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>45583</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>45584</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>45585</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>45586</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>45587</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>45588</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
         <v>45589</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>45590</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>45591</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
         <v>45592</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
         <v>45593</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
         <v>45594</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
         <v>45595</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
         <v>45596</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
         <v>45597</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
         <v>45598</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
         <v>45599</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
         <v>45600</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
         <v>45601</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
         <v>45602</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
         <v>45603</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
         <v>45604</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
         <v>45605</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="6"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
         <v>45606</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="6"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
         <v>45607</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
         <v>45608</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
         <v>45609</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
         <v>45610</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
         <v>45611</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
         <v>45612</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
         <v>45613</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
         <v>45614</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
         <v>45615</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" t="s">
         <v>7</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="6"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
         <v>45616</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="6"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
         <v>45617</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="6"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
         <v>45618</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" t="s">
         <v>10</v>
       </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="6"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="D64" s="4"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
         <v>45619</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="6"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
         <v>45620</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="6"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
         <v>45621</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="6"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
         <v>45622</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="6"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
         <v>45623</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="5"/>
-      <c r="D69" s="6"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="D69" s="4"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
         <v>45624</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" t="s">
         <v>9</v>
       </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="6"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="D70" s="4"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
         <v>45625</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" t="s">
         <v>10</v>
       </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="6"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="D71" s="4"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
         <v>45626</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="6"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
         <v>45627</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" t="s">
         <v>5</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="6"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="D73" s="4"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
         <v>45628</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="6"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="D74" s="4"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
         <v>45629</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="6"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="D75" s="4"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
         <v>45630</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" t="s">
         <v>8</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="6"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+      <c r="D76" s="4"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
         <v>45631</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" t="s">
         <v>9</v>
       </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="6"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+      <c r="D77" s="4"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
         <v>45632</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="6"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
+      <c r="D78" s="4"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
         <v>45633</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="6"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
         <v>45634</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="6"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
         <v>45635</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="6"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
         <v>45636</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" t="s">
         <v>7</v>
       </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="6"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
         <v>45637</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" t="s">
         <v>8</v>
       </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="6"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
         <v>45638</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" t="s">
         <v>9</v>
       </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="6"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+      <c r="D84" s="4"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
         <v>45639</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" t="s">
         <v>10</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="6"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
+      <c r="D85" s="4"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
         <v>45640</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" t="s">
         <v>4</v>
       </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="6"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+      <c r="D86" s="4"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
         <v>45641</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="6"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+      <c r="D87" s="4"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
         <v>45642</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" t="s">
         <v>6</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="6"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+      <c r="D88" s="4"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
         <v>45643</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" t="s">
         <v>7</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="6"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
+      <c r="D89" s="4"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
         <v>45644</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" t="s">
         <v>8</v>
       </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="6"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
+      <c r="D90" s="4"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
         <v>45645</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" t="s">
         <v>9</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="6"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="D91" s="4"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
         <v>45646</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="D92" s="6"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+      <c r="D92" s="4"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
         <v>45647</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" t="s">
         <v>4</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="D93" s="6"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
     </row>
   </sheetData>

</xml_diff>